<commit_message>
listar directorios subir excel
</commit_message>
<xml_diff>
--- a/WebApi.AsambleasDos/Excel/Plantilla_Usuarios_CargaMasiva.xlsx
+++ b/WebApi.AsambleasDos/Excel/Plantilla_Usuarios_CargaMasiva.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t xml:space="preserve"> Teléfono</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>vcoronado</t>
+  </si>
+  <si>
+    <t>vcoronado@saydex.cl</t>
   </si>
 </sst>
 </file>
@@ -410,6 +413,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -428,24 +494,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -462,51 +510,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -837,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,12 +881,12 @@
       <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="8"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -901,44 +904,48 @@
       <c r="E2" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="9" t="s">
+      <c r="G2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="11"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="20"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="14"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="23"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="17"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="32"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G5" s="1"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="20"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -957,177 +964,177 @@
         <v>42</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="5"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="26"/>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="26"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="29"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="14"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="30" t="s">
+      <c r="I9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="32"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="17"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="11"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="20"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="14"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="23"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="29"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="14"/>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="30" t="s">
+      <c r="I13" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="32"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="17"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="11"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="20"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="14"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="23"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="23"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="8"/>
     </row>
     <row r="17" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="23"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="8"/>
     </row>
     <row r="18" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="23"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="8"/>
     </row>
     <row r="19" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="23"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="8"/>
     </row>
     <row r="20" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="23"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="8"/>
     </row>
     <row r="21" spans="7:12" x14ac:dyDescent="0.25">
       <c r="H21" s="1"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="23"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="8"/>
     </row>
     <row r="22" spans="7:12" x14ac:dyDescent="0.25">
       <c r="H22" s="1"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="23"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="8"/>
     </row>
     <row r="23" spans="7:12" x14ac:dyDescent="0.25">
       <c r="H23" s="1"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="23"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="8"/>
     </row>
     <row r="24" spans="7:12" x14ac:dyDescent="0.25">
       <c r="H24" s="1"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="23"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="8"/>
     </row>
     <row r="25" spans="7:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H25" s="1"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="35"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="5"/>
     </row>
     <row r="26" spans="7:12" x14ac:dyDescent="0.25">
       <c r="H26" s="1"/>
@@ -2556,13 +2563,12 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="I25:L25"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="I21:L21"/>
-    <mergeCell ref="I22:L22"/>
-    <mergeCell ref="I23:L23"/>
-    <mergeCell ref="I24:L24"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I5:L5"/>
     <mergeCell ref="I18:L18"/>
     <mergeCell ref="I7:L7"/>
     <mergeCell ref="I8:L8"/>
@@ -2575,20 +2581,22 @@
     <mergeCell ref="I15:L15"/>
     <mergeCell ref="I16:L16"/>
     <mergeCell ref="I17:L17"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="I25:L25"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="I22:L22"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="I24:L24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G6" r:id="rId1" display="jrobrasandrea@gmail.com       4 basico /septimo basico"/>
+    <hyperlink ref="G2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>